<commit_message>
Update SES reproduction (adult and elderly)
</commit_message>
<xml_diff>
--- a/Education & Occupation recode.xlsx
+++ b/Education & Occupation recode.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1660" windowWidth="22300" windowHeight="13180" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="1520" windowWidth="22300" windowHeight="13180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="221">
   <si>
     <t>CFPS egp</t>
   </si>
@@ -331,444 +331,556 @@
   </si>
   <si>
     <t>Lawson, 2013</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1=less than high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2= high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>3 = some college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>4= college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>5 = some graduate level</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>6 = graduate level</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>hanson, 2011</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>5 years=less than six grade</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>11 years= less than high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>12 years= graduated high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>14 years= complete some college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>16 years=college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>17 years= complete some graduate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>19 years= graduate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Ursache, 2016</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>6= &lt;7years of school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>8= 7-9 yrs;</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>10.5= 10-11 yrs;</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>12= high school graduate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>14= some college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>16= college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>18= profestional degree</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Ellwood-Lowe, 2018</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>0= no high school diploma</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2= some college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>5= master's</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>6= doctorate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>CFPS2010eduy_best</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>17= at least one year of postgraduate education</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2 = high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1 = below high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">6 = four-year degree </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">5 = two-year degree </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">3,4 = Techical/Vocational (3); 
 some college (4); </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>7 =MA, PhD, Prefessional</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1 = below high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>5= advanced degree (master &amp; doctorate)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>3= some college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>4 = college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1= less than high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>5= high degree</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2=high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>3= some college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>4= college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>5, part hight school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">4 high school graduate
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">3 part college or post-high school training
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1, post college: master &amp; phd
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">4= high school graduate, 
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">3=bachelor’s degree; 
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Leonard, 2019</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1=lower than college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Ozernov-Palchi, 2019</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1=less than high school
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">4= college
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>5 = some graduate level
 6 = graduate level</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">3= some college
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">17 years= complete some graduate
 19 years= graduate
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">16 years=college
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>6= Less than seven years of school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Noble 2015</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>8 = Seven to nine years of school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>10.5 = Ten to eleven years of school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>12 = High school graduate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>14  = Some college (1-3 years, AA, business schools)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>16 = Four-year college graduate (BA, BS, BM)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>18 = Professional degree (MA, MS, ME, MD, PhD, LLD, JD, etc.)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">4= 4 year college
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>3= 2 year college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1= high school
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">5= master's 6= doctorate
 </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Luby 2013</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">2  high school diploma; </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">3=some college; </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>4 college degree;</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>5  some graduate school or graduate/professional degree]</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1 no high school diplopma;</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Takeuchi, 2019</t>
   </si>
   <si>
     <t>Takeuchi, 2019</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1 &lt;high school diplopma;</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>6, elementary school graduate or below</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>9, junior high school graduate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">11, graduate of a short term school completed after junior high school; </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">12, normal high school graduate; </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>16, university graduate;</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>14, graduate of a short term school completed after high school (such as a junior college);</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">18 Masters degree; </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>21 Doctorate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>18 Masters degree; 21 Doctorate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>PSID edu (years)</t>
   </si>
   <si>
     <t>CFPS2010edu_best/feduc/meduc</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Kong, 2019</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Kong, 2019</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Hair, 2015</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>less than high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>some college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>high school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>some post graduate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>graduate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>High school</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>some college</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>some graduate/graduate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang, 2016</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 = 6 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = 9 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 = 12 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 = 16 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 = 19 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yang,2016</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 = 8 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 = 16 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 = 18 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Johnson, 2013</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Noble,2012b-edu1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Noble,2012b-edu2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>high school or below</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>college or above</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Piras, 2011</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>3=12 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2=9 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1=6 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>4=16 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Piras, 2011</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>5=18 years</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -901,487 +1013,527 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="359">
+  <cellStyleXfs count="375">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="359">
+  <cellStyles count="375">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
@@ -1562,6 +1714,14 @@
     <cellStyle name="超链接" xfId="353" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="355" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="373" builtinId="8" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1741,6 +1901,14 @@
     <cellStyle name="已访问的超链接" xfId="354" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="356" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="374" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1953,10 +2121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1001"/>
+  <dimension ref="A1:Q1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C16"/>
+    <sheetView tabSelected="1" topLeftCell="D53" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Q54" sqref="Q54:Q60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1967,8 +2135,8 @@
     <col min="26" max="16384" width="11.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1995,343 +2163,398 @@
       <c r="I1" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="45" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="28" t="s">
         <v>175</v>
       </c>
       <c r="J2" s="3">
         <v>0</v>
       </c>
-      <c r="K2" s="38"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="K2" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="31">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="23">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="31"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="23"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="23"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="31">
+      <c r="I5" s="28"/>
+      <c r="J5" s="23">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="31"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="K5" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="L5" s="50" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="28"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="23"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="31"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="I7" s="28"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="23"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17" t="s">
+      <c r="E8" s="28"/>
+      <c r="F8" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="28" t="s">
         <v>168</v>
       </c>
       <c r="J8" s="32">
         <v>12</v>
       </c>
-      <c r="K8" s="38"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="K8" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="L8" s="50" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
       <c r="J9" s="32"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="50"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
       <c r="J10" s="32"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="50"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
       <c r="J11" s="32"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="K11" s="29"/>
+      <c r="L11" s="50"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="28">
         <v>2</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="23">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="K12" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="L12" s="50" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18" t="s">
+      <c r="E14" s="28"/>
+      <c r="F14" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="23">
         <v>16</v>
       </c>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="31"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="31"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="28" t="s">
         <v>132</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="17"/>
+      <c r="E17" s="28"/>
       <c r="F17" s="3" t="s">
         <v>100</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="28" t="s">
         <v>171</v>
       </c>
       <c r="J17" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="L17" s="50" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
       <c r="F18" s="3" t="s">
         <v>101</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
       <c r="J18" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="34"/>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>123</v>
       </c>
@@ -2356,216 +2579,271 @@
       <c r="H22" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="I22" s="38" t="s">
+      <c r="I22" s="18" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="K22" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="L22" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>0</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H23" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="I23" s="40" t="s">
+      <c r="I23" s="29" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="K23" s="23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>1</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="40"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>2</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="40"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>3</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="40"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>4</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17" t="s">
+      <c r="B27" s="28"/>
+      <c r="C27" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="40"/>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>5</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="40"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>6</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="40"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>7</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="31" t="s">
+      <c r="G30" s="28"/>
+      <c r="H30" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="I30" s="40"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I30" s="29"/>
+      <c r="J30" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>8</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="40"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>9</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="40"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>10</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="G33" s="29" t="s">
+      <c r="G33" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="H33" s="31" t="s">
+      <c r="H33" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="I33" s="40" t="s">
+      <c r="I33" s="29" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J33" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>11</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>12</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="4" t="s">
         <v>144</v>
       </c>
@@ -2575,29 +2853,36 @@
       <c r="F35" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="G35" s="29"/>
+      <c r="G35" s="41"/>
       <c r="H35" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I35" s="31"/>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I35" s="23"/>
+      <c r="J35" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="K35" s="23"/>
+      <c r="L35" s="24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>13</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="28" t="s">
         <v>160</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -2606,177 +2891,217 @@
       <c r="H36" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="I36" s="41" t="s">
+      <c r="I36" s="46" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J36" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>14</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="3" t="s">
         <v>164</v>
       </c>
       <c r="H37" s="32"/>
-      <c r="I37" s="41"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I37" s="46"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="23">
+        <v>1</v>
+      </c>
+      <c r="L37" s="23"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>15</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="F38" s="17"/>
-      <c r="G38" s="29" t="s">
+      <c r="F38" s="28"/>
+      <c r="G38" s="41" t="s">
         <v>163</v>
       </c>
       <c r="H38" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="I38" s="41" t="s">
+      <c r="I38" s="46" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J38" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>16</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
       <c r="F39" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G39" s="29"/>
+      <c r="G39" s="41"/>
       <c r="H39" s="32"/>
-      <c r="I39" s="41"/>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I39" s="46"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="50" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>17</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G40" s="28" t="s">
         <v>121</v>
       </c>
       <c r="H40" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="I40" s="41" t="s">
+      <c r="I40" s="46" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J40" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>18</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
       <c r="H41" s="32"/>
-      <c r="I41" s="41"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I41" s="46"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>19</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
       <c r="H42" s="32"/>
-      <c r="I42" s="40" t="s">
+      <c r="I42" s="29" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J42" s="28"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>20</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="18" t="s">
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="26" t="s">
         <v>122</v>
       </c>
       <c r="H43" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="I43" s="40"/>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I43" s="29"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>21</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="18"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="26"/>
       <c r="H44" s="32"/>
-      <c r="I44" s="40"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I44" s="29"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>22</v>
       </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="18"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="26"/>
       <c r="H45" s="32"/>
-      <c r="I45" s="40"/>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I45" s="29"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>185</v>
       </c>
@@ -2816,411 +3141,517 @@
       <c r="M53" s="8" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N53" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="O53" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="P53" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q53" s="49" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>0</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D54" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="27" t="s">
+      <c r="E54" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F54" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="G54" s="22" t="s">
+      <c r="G54" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="H54" s="20" t="s">
+      <c r="H54" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="I54" s="22" t="s">
+      <c r="I54" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="J54" s="22" t="s">
+      <c r="J54" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="K54" s="33" t="s">
+      <c r="K54" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="L54" s="39">
+      <c r="L54" s="30">
         <v>6</v>
       </c>
-      <c r="M54" s="39" t="s">
+      <c r="M54" s="30" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N54" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="O54" s="23">
+        <v>0</v>
+      </c>
+      <c r="P54" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q54" s="34" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>1</v>
       </c>
-      <c r="B55" s="20"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
-      <c r="K55" s="33"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="39"/>
-    </row>
-    <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="40"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="30"/>
+      <c r="M55" s="30"/>
+      <c r="N55" s="23"/>
+      <c r="O55" s="23"/>
+      <c r="P55" s="23"/>
+      <c r="Q55" s="23"/>
+    </row>
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>2</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
-      <c r="K56" s="33"/>
-      <c r="L56" s="39"/>
-      <c r="M56" s="39"/>
-    </row>
-    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="40"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="35"/>
+      <c r="L56" s="30"/>
+      <c r="M56" s="30"/>
+      <c r="N56" s="23"/>
+      <c r="O56" s="23"/>
+      <c r="P56" s="23"/>
+      <c r="Q56" s="23"/>
+    </row>
+    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>3</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="39"/>
-      <c r="M57" s="39"/>
-    </row>
-    <row r="58" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="40"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="35"/>
+      <c r="L57" s="30"/>
+      <c r="M57" s="30"/>
+      <c r="N57" s="23"/>
+      <c r="O57" s="23"/>
+      <c r="P57" s="23"/>
+      <c r="Q57" s="23"/>
+    </row>
+    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>4</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="22"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="39"/>
-    </row>
-    <row r="59" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="40"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="30"/>
+      <c r="M58" s="30"/>
+      <c r="N58" s="23"/>
+      <c r="O58" s="23"/>
+      <c r="P58" s="23"/>
+      <c r="Q58" s="23"/>
+    </row>
+    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>5</v>
       </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="39"/>
-    </row>
-    <row r="60" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="40"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="30"/>
+      <c r="M59" s="30"/>
+      <c r="N59" s="23"/>
+      <c r="O59" s="23"/>
+      <c r="P59" s="23"/>
+      <c r="Q59" s="23"/>
+    </row>
+    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>6</v>
       </c>
-      <c r="B60" s="20"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
-    </row>
-    <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="40"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="30"/>
+      <c r="M60" s="30"/>
+      <c r="N60" s="23"/>
+      <c r="O60" s="23"/>
+      <c r="P60" s="23"/>
+      <c r="Q60" s="23"/>
+    </row>
+    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>7</v>
       </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="19" t="s">
+      <c r="B61" s="40"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="F61" s="22"/>
-      <c r="G61" s="19" t="s">
+      <c r="F61" s="37"/>
+      <c r="G61" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="H61" s="23" t="s">
+      <c r="H61" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="I61" s="22"/>
-      <c r="J61" s="22"/>
-      <c r="K61" s="33" t="s">
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="L61" s="39">
+      <c r="L61" s="30">
         <v>8</v>
       </c>
-      <c r="M61" s="39"/>
-    </row>
-    <row r="62" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M61" s="30"/>
+      <c r="N61" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="O61" s="23"/>
+      <c r="P61" s="23"/>
+      <c r="Q61" s="34" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>8</v>
       </c>
-      <c r="B62" s="20"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="23"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="22"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="39"/>
-      <c r="M62" s="39"/>
-    </row>
-    <row r="63" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="40"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="30"/>
+      <c r="M62" s="30"/>
+      <c r="N62" s="23"/>
+      <c r="O62" s="23"/>
+      <c r="P62" s="23"/>
+      <c r="Q62" s="23"/>
+    </row>
+    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>9</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="23" t="s">
+      <c r="D63" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E63" s="19"/>
-      <c r="F63" s="30" t="s">
+      <c r="E63" s="33"/>
+      <c r="F63" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="G63" s="19"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="19" t="s">
+      <c r="G63" s="33"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="J63" s="19" t="s">
+      <c r="J63" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="K63" s="34" t="s">
+      <c r="K63" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="L63" s="39">
+      <c r="L63" s="30">
         <v>12</v>
       </c>
-      <c r="M63" s="39" t="s">
+      <c r="M63" s="30" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N63" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="O63" s="23"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>10</v>
       </c>
-      <c r="B64" s="19"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="25" t="s">
+      <c r="B64" s="33"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="30"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="23" t="s">
+      <c r="F64" s="38"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="I64" s="19"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="34"/>
-      <c r="L64" s="39"/>
-      <c r="M64" s="39"/>
-    </row>
-    <row r="65" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="30"/>
+      <c r="M64" s="30"/>
+      <c r="N64" s="23"/>
+      <c r="O64" s="23"/>
+      <c r="P64" s="23"/>
+      <c r="Q64" s="23"/>
+    </row>
+    <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>11</v>
       </c>
-      <c r="B65" s="19"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="30"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="23"/>
-      <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="34"/>
-      <c r="L65" s="39"/>
-      <c r="M65" s="39"/>
-    </row>
-    <row r="66" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="33"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="39"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="36"/>
+      <c r="L65" s="30"/>
+      <c r="M65" s="30"/>
+      <c r="N65" s="23"/>
+      <c r="O65" s="23"/>
+      <c r="P65" s="23"/>
+      <c r="Q65" s="23"/>
+    </row>
+    <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>12</v>
       </c>
-      <c r="B66" s="19"/>
-      <c r="C66" s="23"/>
-      <c r="D66" s="23"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
       <c r="E66" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F66" s="30"/>
+      <c r="F66" s="38"/>
       <c r="G66" s="8" t="s">
         <v>105</v>
       </c>
       <c r="H66" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33"/>
       <c r="K66" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="L66" s="39"/>
-      <c r="M66" s="39"/>
-    </row>
-    <row r="67" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L66" s="30"/>
+      <c r="M66" s="30"/>
+      <c r="N66" s="23"/>
+      <c r="O66" s="23"/>
+      <c r="P66" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q66" s="23"/>
+    </row>
+    <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>13</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C67" s="23" t="s">
+      <c r="C67" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="D67" s="23" t="s">
+      <c r="D67" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="E67" s="23" t="s">
+      <c r="E67" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="F67" s="23" t="s">
+      <c r="F67" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="G67" s="19" t="s">
+      <c r="G67" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="H67" s="23" t="s">
+      <c r="H67" s="39" t="s">
         <v>160</v>
       </c>
       <c r="I67" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="J67" s="19" t="s">
+      <c r="J67" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="K67" s="34" t="s">
+      <c r="K67" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="L67" s="39">
+      <c r="L67" s="30">
         <v>16</v>
       </c>
-      <c r="M67" s="39" t="s">
+      <c r="M67" s="30" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N67" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="O67" s="23"/>
+      <c r="P67" s="23"/>
+      <c r="Q67" s="34" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>14</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C68" s="23"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="23"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="39"/>
       <c r="I68" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J68" s="19"/>
-      <c r="K68" s="34"/>
-      <c r="L68" s="39"/>
-      <c r="M68" s="39"/>
-    </row>
-    <row r="69" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J68" s="33"/>
+      <c r="K68" s="36"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="30"/>
+      <c r="N68" s="23"/>
+      <c r="O68" s="23">
+        <v>1</v>
+      </c>
+      <c r="P68" s="23"/>
+      <c r="Q68" s="23"/>
+    </row>
+    <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>15</v>
       </c>
-      <c r="B69" s="19" t="s">
+      <c r="B69" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="23" t="s">
+      <c r="C69" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="D69" s="23" t="s">
+      <c r="D69" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="E69" s="23" t="s">
+      <c r="E69" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="F69" s="23" t="s">
+      <c r="F69" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="G69" s="19" t="s">
+      <c r="G69" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="H69" s="23"/>
-      <c r="I69" s="19" t="s">
+      <c r="H69" s="39"/>
+      <c r="I69" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="J69" s="19" t="s">
+      <c r="J69" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="K69" s="34" t="s">
+      <c r="K69" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="L69" s="39"/>
-      <c r="M69" s="42" t="s">
+      <c r="L69" s="30"/>
+      <c r="M69" s="31" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N69" s="23"/>
+      <c r="O69" s="23"/>
+      <c r="P69" s="23"/>
+      <c r="Q69" s="23"/>
+    </row>
+    <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>16</v>
       </c>
-      <c r="B70" s="19"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="19"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="33"/>
       <c r="H70" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="I70" s="19"/>
-      <c r="J70" s="19"/>
-      <c r="K70" s="34"/>
-      <c r="L70" s="39"/>
-      <c r="M70" s="42"/>
-    </row>
-    <row r="71" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I70" s="33"/>
+      <c r="J70" s="33"/>
+      <c r="K70" s="36"/>
+      <c r="L70" s="30"/>
+      <c r="M70" s="31"/>
+      <c r="N70" s="23"/>
+      <c r="O70" s="23"/>
+      <c r="P70" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q70" s="23"/>
+    </row>
+    <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>124</v>
       </c>
@@ -3260,36 +3691,54 @@
       <c r="M71" s="8" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="17"/>
+      <c r="N71" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="O71" s="23"/>
+      <c r="P71" s="24"/>
+      <c r="Q71" s="49" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="28"/>
       <c r="K72" s="5"/>
-    </row>
-    <row r="73" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="17"/>
+      <c r="O72" s="22"/>
+      <c r="P72" s="22"/>
+    </row>
+    <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="28"/>
       <c r="K73" s="5"/>
-    </row>
-    <row r="74" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="17"/>
-      <c r="I74" s="18"/>
+      <c r="O73" s="22"/>
+      <c r="P73" s="22"/>
+    </row>
+    <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="28"/>
+      <c r="I74" s="26"/>
       <c r="K74" s="32"/>
-    </row>
-    <row r="75" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="17"/>
-      <c r="I75" s="18"/>
+      <c r="O74" s="22"/>
+      <c r="P74" s="22"/>
+    </row>
+    <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="28"/>
+      <c r="I75" s="26"/>
       <c r="K75" s="32"/>
-    </row>
-    <row r="76" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="17"/>
-      <c r="I76" s="18"/>
+      <c r="O75" s="22"/>
+      <c r="P75" s="22"/>
+    </row>
+    <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="28"/>
+      <c r="I76" s="26"/>
       <c r="K76" s="32"/>
-    </row>
-    <row r="77" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="17"/>
-    </row>
-    <row r="78" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="O76" s="22"/>
+      <c r="P76" s="22"/>
+    </row>
+    <row r="77" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="28"/>
+    </row>
+    <row r="78" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4212,43 +4661,29 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="143">
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="I23:I32"/>
-    <mergeCell ref="M54:M62"/>
-    <mergeCell ref="M63:M66"/>
-    <mergeCell ref="M67:M68"/>
-    <mergeCell ref="M69:M70"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="L54:L60"/>
-    <mergeCell ref="L61:L62"/>
-    <mergeCell ref="L63:L66"/>
-    <mergeCell ref="L67:L70"/>
-    <mergeCell ref="K74:K76"/>
-    <mergeCell ref="K61:K62"/>
-    <mergeCell ref="K63:K65"/>
-    <mergeCell ref="K54:K60"/>
-    <mergeCell ref="K67:K68"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="J63:J66"/>
-    <mergeCell ref="J69:J70"/>
-    <mergeCell ref="J54:J62"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="I74:I76"/>
-    <mergeCell ref="I54:I62"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="H54:H60"/>
-    <mergeCell ref="H61:H63"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="H67:H69"/>
+  <mergeCells count="177">
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="L12:L16"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="Q54:Q60"/>
+    <mergeCell ref="Q61:Q62"/>
+    <mergeCell ref="Q63:Q66"/>
+    <mergeCell ref="Q67:Q70"/>
+    <mergeCell ref="K12:K16"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="N54:N60"/>
+    <mergeCell ref="N61:N62"/>
+    <mergeCell ref="N63:N66"/>
+    <mergeCell ref="N67:N70"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="G61:G65"/>
+    <mergeCell ref="G54:G60"/>
     <mergeCell ref="H23:H29"/>
     <mergeCell ref="H30:H32"/>
     <mergeCell ref="H33:H34"/>
@@ -4256,30 +4691,60 @@
     <mergeCell ref="H40:H42"/>
     <mergeCell ref="H43:H45"/>
     <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="I8:I11"/>
     <mergeCell ref="I42:I45"/>
     <mergeCell ref="I40:I41"/>
     <mergeCell ref="I38:I39"/>
     <mergeCell ref="I36:I37"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="G61:G65"/>
-    <mergeCell ref="F23:F29"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="F40:F45"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="G23:G32"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="G54:G60"/>
-    <mergeCell ref="F54:F62"/>
-    <mergeCell ref="F63:F66"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B72:B77"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B45"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="B54:B62"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C54:C62"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="E2:E11"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C45"/>
     <mergeCell ref="E12:E18"/>
     <mergeCell ref="E64:E65"/>
     <mergeCell ref="E67:E68"/>
@@ -4303,61 +4768,79 @@
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C45"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="E2:E11"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B72:B77"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="B54:B62"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C54:C62"/>
-    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="F40:F45"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="G23:G32"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="F54:F62"/>
+    <mergeCell ref="F63:F66"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="I74:I76"/>
+    <mergeCell ref="I54:I62"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="H54:H60"/>
+    <mergeCell ref="H61:H63"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="H67:H69"/>
+    <mergeCell ref="K74:K76"/>
+    <mergeCell ref="K61:K62"/>
+    <mergeCell ref="K63:K65"/>
+    <mergeCell ref="K54:K60"/>
+    <mergeCell ref="K67:K68"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="J69:J70"/>
+    <mergeCell ref="J54:J62"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="I23:I32"/>
+    <mergeCell ref="M54:M62"/>
+    <mergeCell ref="M63:M66"/>
+    <mergeCell ref="M67:M68"/>
+    <mergeCell ref="M69:M70"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="L54:L60"/>
+    <mergeCell ref="L61:L62"/>
+    <mergeCell ref="L63:L66"/>
+    <mergeCell ref="L67:L70"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="O54:O67"/>
+    <mergeCell ref="P54:P65"/>
+    <mergeCell ref="P66:P69"/>
+    <mergeCell ref="O68:O71"/>
+    <mergeCell ref="P70:P71"/>
+    <mergeCell ref="J23:J29"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="J40:J45"/>
+    <mergeCell ref="K23:K36"/>
+    <mergeCell ref="K37:K45"/>
+    <mergeCell ref="L23:L34"/>
+    <mergeCell ref="L35:L38"/>
+    <mergeCell ref="L39:L45"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4367,7 +4850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -4445,7 +4928,7 @@
       <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="47" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="15"/>
@@ -4457,7 +4940,7 @@
       <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -5512,7 +5995,7 @@
   <mergeCells count="1">
     <mergeCell ref="C6:C7"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -6593,7 +7076,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -7617,7 +8100,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>